<commit_message>
final plots, still mysterious footprint reduction
</commit_message>
<xml_diff>
--- a/Aggregations/Aggregation_plots.xlsx
+++ b/Aggregations/Aggregation_plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\GT-IOA\Aggregations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MARIO Organization\GreenTechs\Aggregations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D872EE-E863-4AE5-8EC4-92B8420DF5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8578C295-2A97-4DAA-AB13-66B568E10E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Agriculture, cattling &amp; fishering</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Electricity by wind</t>
+  </si>
+  <si>
+    <t>Agriculture &amp; food</t>
+  </si>
+  <si>
+    <t>Petrochemicals</t>
   </si>
 </sst>
 </file>
@@ -159,7 +165,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -440,15 +446,15 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -456,23 +462,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -480,7 +486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -488,7 +494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -496,15 +502,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -512,15 +518,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -528,7 +534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -536,7 +542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -544,7 +550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -552,7 +558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -560,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -568,7 +574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -576,7 +582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -584,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -592,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -600,7 +606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -608,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -616,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -624,7 +630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>

</xml_diff>